<commit_message>
Changed conceptAlias to conceptUri in deepRoots.lookup method Changed dwc:Event to http://purl.org/dc/dcmitype/Event in indoPacificConfiguration.xml file
</commit_message>
<xml_diff>
--- a/sampledata/Apogon_indoPacificTemplate_v3.xlsx
+++ b/sampledata/Apogon_indoPacificTemplate_v3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -916,9 +916,6 @@
     <t xml:space="preserve">HER_97 </t>
   </si>
   <si>
-    <t xml:space="preserve">HER_98 </t>
-  </si>
-  <si>
     <t xml:space="preserve">HER_99 </t>
   </si>
   <si>
@@ -1274,6 +1271,9 @@
   </si>
   <si>
     <t>sex</t>
+  </si>
+  <si>
+    <t>HER_98</t>
   </si>
 </sst>
 </file>
@@ -1906,17 +1906,17 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
         <v>104</v>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
         <v>105</v>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>106</v>
@@ -1940,22 +1940,22 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
         <v>107</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B11" t="s">
         <v>108</v>
@@ -1971,17 +1971,17 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" t="s">
         <v>109</v>
@@ -1989,7 +1989,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" t="s">
         <v>90</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
         <v>90</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
         <v>92</v>
@@ -2016,12 +2016,12 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -2029,27 +2029,27 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24" t="s">
         <v>57</v>
@@ -2057,147 +2057,147 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2215,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2239,160 +2239,160 @@
   <sheetData>
     <row r="1" spans="1:52" s="16" customFormat="1">
       <c r="A1" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="S1" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="R1" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="U1" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="T1" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="W1" s="14" t="s">
+      <c r="X1" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="X1" s="14" t="s">
+      <c r="Y1" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AA1" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AB1" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AC1" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AD1" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AE1" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AF1" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AG1" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AH1" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AI1" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AK1" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AL1" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AT1" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="AT1" s="11" t="s">
+      <c r="AU1" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="AU1" s="11" t="s">
+      <c r="AV1" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="AV1" s="11" t="s">
+      <c r="AW1" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="AW1" s="11" t="s">
+      <c r="AX1" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="AX1" s="11" t="s">
+      <c r="AY1" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="AY1" s="11" t="s">
+      <c r="AZ1" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="AZ1" s="11" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:52">
@@ -2400,7 +2400,7 @@
         <v>110</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>103</v>
@@ -2430,13 +2430,13 @@
         <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>95</v>
@@ -2495,7 +2495,7 @@
       </c>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ2" s="1"/>
       <c r="AK2" s="1"/>
@@ -2504,10 +2504,10 @@
         <v>46</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP2" s="1" t="s">
         <v>101</v>
@@ -2538,7 +2538,7 @@
         <v>111</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>103</v>
@@ -2571,10 +2571,10 @@
         <v>49</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
@@ -2602,7 +2602,7 @@
         <v>0</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y3" s="1" t="s">
         <v>95</v>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
@@ -2642,10 +2642,10 @@
         <v>46</v>
       </c>
       <c r="AN3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP3" s="1" t="s">
         <v>101</v>
@@ -2676,7 +2676,7 @@
         <v>112</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>103</v>
@@ -2709,10 +2709,10 @@
         <v>49</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
@@ -2740,7 +2740,7 @@
         <v>0</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>95</v>
@@ -2771,7 +2771,7 @@
       </c>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
@@ -2780,10 +2780,10 @@
         <v>46</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP4" s="1" t="s">
         <v>101</v>
@@ -2814,7 +2814,7 @@
         <v>113</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>103</v>
@@ -2847,10 +2847,10 @@
         <v>49</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
@@ -2878,7 +2878,7 @@
         <v>0</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y5" s="1" t="s">
         <v>95</v>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
@@ -2918,10 +2918,10 @@
         <v>46</v>
       </c>
       <c r="AN5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP5" s="1" t="s">
         <v>101</v>
@@ -2949,10 +2949,10 @@
     </row>
     <row r="6" spans="1:52">
       <c r="A6" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>103</v>
@@ -2985,10 +2985,10 @@
         <v>49</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
@@ -3016,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>95</v>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ6" s="1"/>
       <c r="AK6" s="1"/>
@@ -3056,10 +3056,10 @@
         <v>46</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP6" s="1" t="s">
         <v>101</v>
@@ -3087,10 +3087,10 @@
     </row>
     <row r="7" spans="1:52">
       <c r="A7" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>103</v>
@@ -3123,10 +3123,10 @@
         <v>49</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1" t="s">
@@ -3154,7 +3154,7 @@
         <v>0</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>95</v>
@@ -3185,7 +3185,7 @@
       </c>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ7" s="1"/>
       <c r="AK7" s="1"/>
@@ -3194,10 +3194,10 @@
         <v>46</v>
       </c>
       <c r="AN7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP7" s="1" t="s">
         <v>101</v>
@@ -3228,7 +3228,7 @@
         <v>114</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>103</v>
@@ -3261,10 +3261,10 @@
         <v>49</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>95</v>
@@ -3323,7 +3323,7 @@
       </c>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ8" s="1"/>
       <c r="AK8" s="1"/>
@@ -3332,10 +3332,10 @@
         <v>46</v>
       </c>
       <c r="AN8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP8" s="1" t="s">
         <v>101</v>
@@ -3366,7 +3366,7 @@
         <v>115</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>103</v>
@@ -3399,10 +3399,10 @@
         <v>49</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1" t="s">
@@ -3430,7 +3430,7 @@
         <v>0</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y9" s="1" t="s">
         <v>95</v>
@@ -3461,7 +3461,7 @@
       </c>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
@@ -3470,10 +3470,10 @@
         <v>46</v>
       </c>
       <c r="AN9" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO9" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP9" s="1" t="s">
         <v>101</v>
@@ -3504,7 +3504,7 @@
         <v>116</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>103</v>
@@ -3537,10 +3537,10 @@
         <v>49</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
@@ -3568,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>95</v>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ10" s="1"/>
       <c r="AK10" s="1"/>
@@ -3608,10 +3608,10 @@
         <v>46</v>
       </c>
       <c r="AN10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP10" s="1" t="s">
         <v>101</v>
@@ -3642,7 +3642,7 @@
         <v>117</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>103</v>
@@ -3675,10 +3675,10 @@
         <v>49</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
@@ -3706,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>95</v>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ11" s="1"/>
       <c r="AK11" s="1"/>
@@ -3746,10 +3746,10 @@
         <v>46</v>
       </c>
       <c r="AN11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP11" s="1" t="s">
         <v>101</v>
@@ -3780,7 +3780,7 @@
         <v>118</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>103</v>
@@ -3813,10 +3813,10 @@
         <v>49</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>95</v>
@@ -3875,7 +3875,7 @@
       </c>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
@@ -3884,10 +3884,10 @@
         <v>46</v>
       </c>
       <c r="AN12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP12" s="1" t="s">
         <v>101</v>
@@ -3918,7 +3918,7 @@
         <v>119</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>103</v>
@@ -3951,10 +3951,10 @@
         <v>49</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
@@ -3982,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>95</v>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ13" s="1"/>
       <c r="AK13" s="1"/>
@@ -4022,10 +4022,10 @@
         <v>46</v>
       </c>
       <c r="AN13" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO13" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP13" s="1" t="s">
         <v>101</v>
@@ -4056,7 +4056,7 @@
         <v>120</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>103</v>
@@ -4089,10 +4089,10 @@
         <v>49</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
@@ -4120,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>95</v>
@@ -4151,7 +4151,7 @@
       </c>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ14" s="1"/>
       <c r="AK14" s="1"/>
@@ -4160,10 +4160,10 @@
         <v>46</v>
       </c>
       <c r="AN14" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO14" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP14" s="1" t="s">
         <v>101</v>
@@ -4191,10 +4191,10 @@
     </row>
     <row r="15" spans="1:52">
       <c r="A15" s="1" t="s">
-        <v>121</v>
+        <v>240</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>103</v>
@@ -4227,10 +4227,10 @@
         <v>49</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
@@ -4258,7 +4258,7 @@
         <v>0</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y15" s="1" t="s">
         <v>95</v>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
@@ -4298,10 +4298,10 @@
         <v>46</v>
       </c>
       <c r="AN15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO15" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP15" s="1" t="s">
         <v>101</v>
@@ -4329,10 +4329,10 @@
     </row>
     <row r="16" spans="1:52">
       <c r="A16" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>103</v>
@@ -4365,10 +4365,10 @@
         <v>49</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1" t="s">
@@ -4396,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y16" s="1" t="s">
         <v>95</v>
@@ -4427,7 +4427,7 @@
       </c>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
@@ -4436,10 +4436,10 @@
         <v>46</v>
       </c>
       <c r="AN16" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO16" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP16" s="1" t="s">
         <v>101</v>
@@ -4467,10 +4467,10 @@
     </row>
     <row r="17" spans="1:52">
       <c r="A17" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>103</v>
@@ -4503,10 +4503,10 @@
         <v>50</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1" t="s">
@@ -4528,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y17" s="1" t="s">
         <v>95</v>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ17" s="1"/>
       <c r="AK17" s="1"/>
@@ -4568,10 +4568,10 @@
         <v>53</v>
       </c>
       <c r="AN17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO17" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP17" s="1" t="s">
         <v>101</v>
@@ -4602,7 +4602,7 @@
         <v>61</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>103</v>
@@ -4635,10 +4635,10 @@
         <v>50</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1" t="s">
@@ -4660,7 +4660,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y18" s="1" t="s">
         <v>95</v>
@@ -4691,7 +4691,7 @@
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
@@ -4700,10 +4700,10 @@
         <v>53</v>
       </c>
       <c r="AN18" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO18" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP18" s="1" t="s">
         <v>101</v>
@@ -4734,7 +4734,7 @@
         <v>62</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>103</v>
@@ -4767,10 +4767,10 @@
         <v>50</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1" t="s">
@@ -4792,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y19" s="1" t="s">
         <v>95</v>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ19" s="1"/>
       <c r="AK19" s="1"/>
@@ -4832,10 +4832,10 @@
         <v>53</v>
       </c>
       <c r="AN19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO19" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP19" s="1" t="s">
         <v>101</v>
@@ -4866,7 +4866,7 @@
         <v>63</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>103</v>
@@ -4899,10 +4899,10 @@
         <v>50</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
@@ -4924,7 +4924,7 @@
         <v>0</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y20" s="1" t="s">
         <v>95</v>
@@ -4955,7 +4955,7 @@
       </c>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ20" s="1"/>
       <c r="AK20" s="1"/>
@@ -4964,10 +4964,10 @@
         <v>53</v>
       </c>
       <c r="AN20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP20" s="1" t="s">
         <v>101</v>
@@ -4998,7 +4998,7 @@
         <v>64</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>103</v>
@@ -5031,10 +5031,10 @@
         <v>50</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1" t="s">
@@ -5056,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y21" s="1" t="s">
         <v>95</v>
@@ -5087,7 +5087,7 @@
       </c>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
@@ -5096,10 +5096,10 @@
         <v>53</v>
       </c>
       <c r="AN21" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO21" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP21" s="1" t="s">
         <v>101</v>
@@ -5130,7 +5130,7 @@
         <v>65</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>103</v>
@@ -5163,10 +5163,10 @@
         <v>50</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
@@ -5188,7 +5188,7 @@
         <v>0</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y22" s="1" t="s">
         <v>95</v>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
@@ -5228,10 +5228,10 @@
         <v>53</v>
       </c>
       <c r="AN22" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO22" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP22" s="1" t="s">
         <v>101</v>
@@ -5262,7 +5262,7 @@
         <v>66</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>103</v>
@@ -5295,10 +5295,10 @@
         <v>50</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1" t="s">
@@ -5320,7 +5320,7 @@
         <v>0</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y23" s="1" t="s">
         <v>95</v>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="AH23" s="1"/>
       <c r="AI23" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
@@ -5360,10 +5360,10 @@
         <v>53</v>
       </c>
       <c r="AN23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP23" s="1" t="s">
         <v>101</v>
@@ -5394,7 +5394,7 @@
         <v>67</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>103</v>
@@ -5427,10 +5427,10 @@
         <v>50</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
@@ -5452,7 +5452,7 @@
         <v>0</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y24" s="1" t="s">
         <v>95</v>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="AH24" s="1"/>
       <c r="AI24" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
@@ -5492,10 +5492,10 @@
         <v>53</v>
       </c>
       <c r="AN24" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO24" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP24" s="1" t="s">
         <v>101</v>
@@ -5526,7 +5526,7 @@
         <v>68</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>103</v>
@@ -5559,10 +5559,10 @@
         <v>50</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
@@ -5584,7 +5584,7 @@
         <v>0</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y25" s="1" t="s">
         <v>95</v>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
@@ -5624,10 +5624,10 @@
         <v>53</v>
       </c>
       <c r="AN25" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO25" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP25" s="1" t="s">
         <v>101</v>
@@ -5658,7 +5658,7 @@
         <v>69</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>103</v>
@@ -5691,10 +5691,10 @@
         <v>50</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1" t="s">
@@ -5716,7 +5716,7 @@
         <v>0</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y26" s="1" t="s">
         <v>95</v>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
@@ -5756,10 +5756,10 @@
         <v>53</v>
       </c>
       <c r="AN26" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO26" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP26" s="1" t="s">
         <v>101</v>
@@ -5790,7 +5790,7 @@
         <v>70</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>103</v>
@@ -5823,10 +5823,10 @@
         <v>50</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1" t="s">
@@ -5848,7 +5848,7 @@
         <v>0</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y27" s="1" t="s">
         <v>95</v>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
@@ -5888,10 +5888,10 @@
         <v>53</v>
       </c>
       <c r="AN27" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO27" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP27" s="1" t="s">
         <v>101</v>
@@ -5922,7 +5922,7 @@
         <v>71</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>103</v>
@@ -5958,7 +5958,7 @@
         <v>55</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
@@ -5985,7 +5985,7 @@
         <v>0</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y28" s="1" t="s">
         <v>60</v>
@@ -6016,7 +6016,7 @@
       </c>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
@@ -6025,10 +6025,10 @@
         <v>46</v>
       </c>
       <c r="AN28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO28" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP28" s="1" t="s">
         <v>58</v>
@@ -6059,7 +6059,7 @@
         <v>72</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>103</v>
@@ -6095,7 +6095,7 @@
         <v>55</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
@@ -6122,7 +6122,7 @@
         <v>0</v>
       </c>
       <c r="X29" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>60</v>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
@@ -6162,10 +6162,10 @@
         <v>46</v>
       </c>
       <c r="AN29" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO29" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP29" s="1" t="s">
         <v>58</v>
@@ -6196,7 +6196,7 @@
         <v>73</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>103</v>
@@ -6232,7 +6232,7 @@
         <v>55</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1" t="s">
@@ -6259,7 +6259,7 @@
         <v>0</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y30" s="1" t="s">
         <v>60</v>
@@ -6290,7 +6290,7 @@
       </c>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
@@ -6299,10 +6299,10 @@
         <v>46</v>
       </c>
       <c r="AN30" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO30" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP30" s="1" t="s">
         <v>58</v>
@@ -6333,7 +6333,7 @@
         <v>74</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>103</v>
@@ -6369,7 +6369,7 @@
         <v>55</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1" t="s">
@@ -6396,7 +6396,7 @@
         <v>0</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y31" s="1" t="s">
         <v>60</v>
@@ -6427,7 +6427,7 @@
       </c>
       <c r="AH31" s="1"/>
       <c r="AI31" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
@@ -6436,10 +6436,10 @@
         <v>46</v>
       </c>
       <c r="AN31" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO31" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP31" s="1" t="s">
         <v>58</v>
@@ -6470,7 +6470,7 @@
         <v>75</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>103</v>
@@ -6506,7 +6506,7 @@
         <v>55</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1" t="s">
@@ -6533,7 +6533,7 @@
         <v>0</v>
       </c>
       <c r="X32" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y32" s="1" t="s">
         <v>60</v>
@@ -6564,7 +6564,7 @@
       </c>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
@@ -6573,10 +6573,10 @@
         <v>46</v>
       </c>
       <c r="AN32" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO32" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP32" s="1" t="s">
         <v>58</v>
@@ -6607,7 +6607,7 @@
         <v>76</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>103</v>
@@ -6643,7 +6643,7 @@
         <v>55</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1" t="s">
@@ -6670,7 +6670,7 @@
         <v>0</v>
       </c>
       <c r="X33" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y33" s="1" t="s">
         <v>60</v>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
@@ -6710,10 +6710,10 @@
         <v>46</v>
       </c>
       <c r="AN33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO33" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP33" s="1" t="s">
         <v>58</v>
@@ -6744,7 +6744,7 @@
         <v>77</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>103</v>
@@ -6780,7 +6780,7 @@
         <v>55</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1" t="s">
@@ -6807,7 +6807,7 @@
         <v>0</v>
       </c>
       <c r="X34" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y34" s="1" t="s">
         <v>60</v>
@@ -6838,7 +6838,7 @@
       </c>
       <c r="AH34" s="1"/>
       <c r="AI34" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ34" s="1"/>
       <c r="AK34" s="1"/>
@@ -6847,10 +6847,10 @@
         <v>46</v>
       </c>
       <c r="AN34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO34" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP34" s="1" t="s">
         <v>58</v>
@@ -6881,7 +6881,7 @@
         <v>78</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>103</v>
@@ -6917,7 +6917,7 @@
         <v>55</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1" t="s">
@@ -6944,7 +6944,7 @@
         <v>0</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y35" s="1" t="s">
         <v>60</v>
@@ -6975,7 +6975,7 @@
       </c>
       <c r="AH35" s="1"/>
       <c r="AI35" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ35" s="1"/>
       <c r="AK35" s="1"/>
@@ -6984,10 +6984,10 @@
         <v>46</v>
       </c>
       <c r="AN35" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO35" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP35" s="1" t="s">
         <v>58</v>
@@ -7018,7 +7018,7 @@
         <v>79</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>103</v>
@@ -7054,7 +7054,7 @@
         <v>55</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1" t="s">
@@ -7081,7 +7081,7 @@
         <v>0</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y36" s="1" t="s">
         <v>60</v>
@@ -7112,7 +7112,7 @@
       </c>
       <c r="AH36" s="1"/>
       <c r="AI36" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
@@ -7121,10 +7121,10 @@
         <v>46</v>
       </c>
       <c r="AN36" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO36" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP36" s="1" t="s">
         <v>58</v>
@@ -7155,7 +7155,7 @@
         <v>80</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>103</v>
@@ -7191,7 +7191,7 @@
         <v>55</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1" t="s">
@@ -7218,7 +7218,7 @@
         <v>0</v>
       </c>
       <c r="X37" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y37" s="1" t="s">
         <v>60</v>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="AH37" s="1"/>
       <c r="AI37" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="1"/>
@@ -7258,10 +7258,10 @@
         <v>46</v>
       </c>
       <c r="AN37" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO37" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP37" s="1" t="s">
         <v>58</v>
@@ -7292,7 +7292,7 @@
         <v>81</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>103</v>
@@ -7328,7 +7328,7 @@
         <v>55</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1" t="s">
@@ -7355,7 +7355,7 @@
         <v>0</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y38" s="1" t="s">
         <v>60</v>
@@ -7386,7 +7386,7 @@
       </c>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
@@ -7395,10 +7395,10 @@
         <v>46</v>
       </c>
       <c r="AN38" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO38" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP38" s="1" t="s">
         <v>58</v>
@@ -7429,7 +7429,7 @@
         <v>82</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>103</v>
@@ -7465,7 +7465,7 @@
         <v>55</v>
       </c>
       <c r="N39" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1" t="s">
@@ -7492,7 +7492,7 @@
         <v>0</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y39" s="1" t="s">
         <v>60</v>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ39" s="1"/>
       <c r="AK39" s="1"/>
@@ -7532,10 +7532,10 @@
         <v>46</v>
       </c>
       <c r="AN39" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO39" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP39" s="1" t="s">
         <v>58</v>
@@ -7566,7 +7566,7 @@
         <v>83</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>103</v>
@@ -7602,7 +7602,7 @@
         <v>55</v>
       </c>
       <c r="N40" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1" t="s">
@@ -7629,7 +7629,7 @@
         <v>0</v>
       </c>
       <c r="X40" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y40" s="1" t="s">
         <v>60</v>
@@ -7660,7 +7660,7 @@
       </c>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
@@ -7669,10 +7669,10 @@
         <v>46</v>
       </c>
       <c r="AN40" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO40" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP40" s="1" t="s">
         <v>58</v>
@@ -7703,7 +7703,7 @@
         <v>84</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>103</v>
@@ -7739,7 +7739,7 @@
         <v>55</v>
       </c>
       <c r="N41" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1" t="s">
@@ -7766,7 +7766,7 @@
         <v>0</v>
       </c>
       <c r="X41" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y41" s="1" t="s">
         <v>60</v>
@@ -7797,7 +7797,7 @@
       </c>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ41" s="1"/>
       <c r="AK41" s="1"/>
@@ -7806,10 +7806,10 @@
         <v>46</v>
       </c>
       <c r="AN41" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO41" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP41" s="1" t="s">
         <v>58</v>
@@ -7840,7 +7840,7 @@
         <v>85</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>103</v>
@@ -7876,7 +7876,7 @@
         <v>55</v>
       </c>
       <c r="N42" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1" t="s">
@@ -7903,7 +7903,7 @@
         <v>0</v>
       </c>
       <c r="X42" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y42" s="1" t="s">
         <v>60</v>
@@ -7934,7 +7934,7 @@
       </c>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ42" s="1"/>
       <c r="AK42" s="1"/>
@@ -7943,10 +7943,10 @@
         <v>46</v>
       </c>
       <c r="AN42" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO42" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP42" s="1" t="s">
         <v>58</v>
@@ -7977,7 +7977,7 @@
         <v>86</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>103</v>
@@ -8013,7 +8013,7 @@
         <v>55</v>
       </c>
       <c r="N43" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1" t="s">
@@ -8040,7 +8040,7 @@
         <v>0</v>
       </c>
       <c r="X43" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y43" s="1" t="s">
         <v>60</v>
@@ -8071,7 +8071,7 @@
       </c>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ43" s="1"/>
       <c r="AK43" s="1"/>
@@ -8080,10 +8080,10 @@
         <v>46</v>
       </c>
       <c r="AN43" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO43" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP43" s="1" t="s">
         <v>58</v>
@@ -8114,7 +8114,7 @@
         <v>87</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>103</v>
@@ -8150,7 +8150,7 @@
         <v>55</v>
       </c>
       <c r="N44" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
@@ -8177,7 +8177,7 @@
         <v>0</v>
       </c>
       <c r="X44" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y44" s="1" t="s">
         <v>60</v>
@@ -8208,7 +8208,7 @@
       </c>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ44" s="1"/>
       <c r="AK44" s="1"/>
@@ -8217,10 +8217,10 @@
         <v>46</v>
       </c>
       <c r="AN44" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO44" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP44" s="1" t="s">
         <v>58</v>
@@ -8251,7 +8251,7 @@
         <v>88</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>103</v>
@@ -8287,7 +8287,7 @@
         <v>55</v>
       </c>
       <c r="N45" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1" t="s">
@@ -8314,7 +8314,7 @@
         <v>0</v>
       </c>
       <c r="X45" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Y45" s="1" t="s">
         <v>60</v>
@@ -8345,7 +8345,7 @@
       </c>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AJ45" s="1"/>
       <c r="AK45" s="1"/>
@@ -8354,10 +8354,10 @@
         <v>46</v>
       </c>
       <c r="AN45" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AO45" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AP45" s="1" t="s">
         <v>58</v>
@@ -8451,51 +8451,51 @@
   <sheetData>
     <row r="1" spans="2:10" s="13" customFormat="1">
       <c r="B1" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D1" s="10"/>
       <c r="E1" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="2:10">
       <c r="B2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("&lt;field&gt;",C2,"&lt;/field&gt;")</f>
         <v>&lt;field&gt;CAS&lt;/field&gt;</v>
       </c>
       <c r="E2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE("&lt;field&gt;",$E2,"&lt;/field&gt;")</f>
         <v>&lt;field&gt;Red Sea and Gulf of Aden&lt;/field&gt;</v>
       </c>
       <c r="G2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H2" t="str">
         <f t="shared" ref="H2:H13" si="0">CONCATENATE("&lt;field&gt;",$G2,"&lt;/field&gt;")</f>
         <v>&lt;field&gt;Coral Reef&lt;/field&gt;</v>
       </c>
       <c r="I2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J7" si="1">CONCATENATE("&lt;field&gt;",$I2,"&lt;/field&gt;")</f>
@@ -8504,31 +8504,31 @@
     </row>
     <row r="3" spans="2:10">
       <c r="B3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D12" si="2">CONCATENATE("&lt;field&gt;",C3,"&lt;/field&gt;")</f>
         <v>&lt;field&gt;IBRC&lt;/field&gt;</v>
       </c>
       <c r="E3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F26" si="3">CONCATENATE("&lt;field&gt;",$E3,"&lt;/field&gt;")</f>
         <v>&lt;field&gt;Somali/Arabian&lt;/field&gt;</v>
       </c>
       <c r="G3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
         <v>&lt;field&gt;Intertidal&lt;/field&gt;</v>
       </c>
       <c r="I3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J3" t="str">
         <f t="shared" si="1"/>
@@ -8537,28 +8537,28 @@
     </row>
     <row r="4" spans="2:10">
       <c r="C4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;KAUST&lt;/field&gt;</v>
       </c>
       <c r="E4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Western Indian Ocean&lt;/field&gt;</v>
       </c>
       <c r="G4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
         <v>&lt;field&gt;Fouling&lt;/field&gt;</v>
       </c>
       <c r="I4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="1"/>
@@ -8567,28 +8567,28 @@
     </row>
     <row r="5" spans="2:10">
       <c r="C5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;ODU&lt;/field&gt;</v>
       </c>
       <c r="E5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;West and South Indian Shelf&lt;/field&gt;</v>
       </c>
       <c r="G5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
         <v>&lt;field&gt;Macroalgae&lt;/field&gt;</v>
       </c>
       <c r="I5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
@@ -8597,28 +8597,28 @@
     </row>
     <row r="6" spans="2:10">
       <c r="C6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;StellenboschU&lt;/field&gt;</v>
       </c>
       <c r="E6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Central Indian Ocean Islands&lt;/field&gt;</v>
       </c>
       <c r="G6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
         <v>&lt;field&gt;Mangrove&lt;/field&gt;</v>
       </c>
       <c r="I6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
@@ -8627,28 +8627,28 @@
     </row>
     <row r="7" spans="2:10">
       <c r="C7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;STRI&lt;/field&gt;</v>
       </c>
       <c r="E7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Bay of Bengal&lt;/field&gt;</v>
       </c>
       <c r="G7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
         <v>&lt;field&gt;Mud&lt;/field&gt;</v>
       </c>
       <c r="I7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="1"/>
@@ -8657,21 +8657,21 @@
     </row>
     <row r="8" spans="2:10">
       <c r="C8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;TAMU&lt;/field&gt;</v>
       </c>
       <c r="E8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Andaman&lt;/field&gt;</v>
       </c>
       <c r="G8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -8680,21 +8680,21 @@
     </row>
     <row r="9" spans="2:10">
       <c r="C9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;UCLA&lt;/field&gt;</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;South China Sea&lt;/field&gt;</v>
       </c>
       <c r="G9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -8703,21 +8703,21 @@
     </row>
     <row r="10" spans="2:10">
       <c r="C10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;UH&lt;/field&gt;</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Sunda Shelf&lt;/field&gt;</v>
       </c>
       <c r="G10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -8726,21 +8726,21 @@
     </row>
     <row r="11" spans="2:10">
       <c r="C11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;UPMSI&lt;/field&gt;</v>
       </c>
       <c r="E11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Java Transitional&lt;/field&gt;</v>
       </c>
       <c r="G11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -8749,21 +8749,21 @@
     </row>
     <row r="12" spans="2:10">
       <c r="C12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="2"/>
         <v>&lt;field&gt;UQ&lt;/field&gt;</v>
       </c>
       <c r="E12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;South Kuroshio&lt;/field&gt;</v>
       </c>
       <c r="G12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -8772,14 +8772,14 @@
     </row>
     <row r="13" spans="2:10">
       <c r="E13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="3"/>
         <v>&lt;field&gt;Tropical Northwestern Pacific&lt;/field&gt;</v>
       </c>
       <c r="G13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -8788,7 +8788,7 @@
     </row>
     <row r="14" spans="2:10">
       <c r="E14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="3"/>
@@ -8797,7 +8797,7 @@
     </row>
     <row r="15" spans="2:10">
       <c r="E15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="3"/>
@@ -8806,7 +8806,7 @@
     </row>
     <row r="16" spans="2:10">
       <c r="E16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="3"/>
@@ -8815,7 +8815,7 @@
     </row>
     <row r="17" spans="5:6">
       <c r="E17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="3"/>
@@ -8824,7 +8824,7 @@
     </row>
     <row r="18" spans="5:6">
       <c r="E18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="3"/>
@@ -8833,7 +8833,7 @@
     </row>
     <row r="19" spans="5:6">
       <c r="E19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="3"/>
@@ -8842,7 +8842,7 @@
     </row>
     <row r="20" spans="5:6">
       <c r="E20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="3"/>
@@ -8851,7 +8851,7 @@
     </row>
     <row r="21" spans="5:6">
       <c r="E21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="3"/>
@@ -8860,7 +8860,7 @@
     </row>
     <row r="22" spans="5:6">
       <c r="E22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="3"/>
@@ -8869,7 +8869,7 @@
     </row>
     <row r="23" spans="5:6">
       <c r="E23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="3"/>
@@ -8878,7 +8878,7 @@
     </row>
     <row r="24" spans="5:6">
       <c r="E24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="3"/>
@@ -8887,7 +8887,7 @@
     </row>
     <row r="25" spans="5:6">
       <c r="E25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="3"/>
@@ -8896,7 +8896,7 @@
     </row>
     <row r="26" spans="5:6">
       <c r="E26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="3"/>

</xml_diff>